<commit_message>
added an input and output text box. Changed the thread to Await instead of wait.
</commit_message>
<xml_diff>
--- a/packages/Data/gild/gildBag.xlsx
+++ b/packages/Data/gild/gildBag.xlsx
@@ -24,7 +24,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+  <si>
+    <t>Date/Time</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>elapsedMs</t>
+  </si>
+  <si>
+    <t>wordCount</t>
+  </si>
+  <si>
+    <t>sentenceCount</t>
+  </si>
+  <si>
+    <t>posWordCount</t>
+  </si>
+  <si>
+    <t>negWordCount</t>
+  </si>
+  <si>
+    <t>posWordPercentage</t>
+  </si>
+  <si>
+    <t>negWordPercentage</t>
+  </si>
+  <si>
+    <t>posPhraseCount</t>
+  </si>
+  <si>
+    <t>negativePhraseCount</t>
+  </si>
+  <si>
+    <t>negPhrasePercentage</t>
+  </si>
   <si>
     <t>Bag</t>
   </si>
@@ -345,51 +381,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42583.9371875</v>
+        <v>42585.690983796296</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>9547</v>
+        <v>8286</v>
       </c>
       <c r="D2">
-        <v>15018</v>
+        <v>13068</v>
       </c>
       <c r="E2">
-        <v>1781</v>
+        <v>1529</v>
       </c>
       <c r="F2">
-        <v>298</v>
+        <v>227</v>
       </c>
       <c r="G2">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="H2">
         <v>65</v>
       </c>
       <c r="I2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>65</v>
       </c>
       <c r="M2">
-        <v>60</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42585.694803240738</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>8277</v>
+      </c>
+      <c r="D3">
+        <v>13180</v>
+      </c>
+      <c r="E3">
+        <v>1559</v>
+      </c>
+      <c r="F3">
+        <v>231</v>
+      </c>
+      <c r="G3">
+        <v>114</v>
+      </c>
+      <c r="H3">
+        <v>64</v>
+      </c>
+      <c r="I3">
+        <v>31</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>64</v>
+      </c>
+      <c r="M3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42585.698263888888</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>8157</v>
+      </c>
+      <c r="D4">
+        <v>13177</v>
+      </c>
+      <c r="E4">
+        <v>1559</v>
+      </c>
+      <c r="F4">
+        <v>230</v>
+      </c>
+      <c r="G4">
+        <v>114</v>
+      </c>
+      <c r="H4">
+        <v>66</v>
+      </c>
+      <c r="I4">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>66</v>
+      </c>
+      <c r="M4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42585.704293981478</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>8262</v>
+      </c>
+      <c r="D5">
+        <v>13187</v>
+      </c>
+      <c r="E5">
+        <v>1540</v>
+      </c>
+      <c r="F5">
+        <v>230</v>
+      </c>
+      <c r="G5">
+        <v>116</v>
+      </c>
+      <c r="H5">
+        <v>64</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>64</v>
+      </c>
+      <c r="M5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42585.70722222222</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>8494</v>
+      </c>
+      <c r="D6">
+        <v>13313</v>
+      </c>
+      <c r="E6">
+        <v>1571</v>
+      </c>
+      <c r="F6">
+        <v>234</v>
+      </c>
+      <c r="G6">
+        <v>115</v>
+      </c>
+      <c r="H6">
+        <v>65</v>
+      </c>
+      <c r="I6">
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>65</v>
+      </c>
+      <c r="M6">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>